<commit_message>
Commit on 28th May 2024
</commit_message>
<xml_diff>
--- a/Auto-IT/bulk_clients.xlsx
+++ b/Auto-IT/bulk_clients.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15530" windowHeight="6730"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13450" windowHeight="5860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="D1:L17"/>
 </workbook>
 </file>
 
@@ -70,15 +66,9 @@
     <t>seed.co</t>
   </si>
   <si>
-    <t>laddu</t>
-  </si>
-  <si>
     <t>Inactive</t>
   </si>
   <si>
-    <t>jv colony</t>
-  </si>
-  <si>
     <t>Gachibowli</t>
   </si>
   <si>
@@ -94,21 +84,12 @@
     <t>Eastern Cape</t>
   </si>
   <si>
-    <t>gouti@gmail.com</t>
-  </si>
-  <si>
     <t>earth.co</t>
   </si>
   <si>
-    <t>garuda</t>
-  </si>
-  <si>
     <t>active</t>
   </si>
   <si>
-    <t>siddque</t>
-  </si>
-  <si>
     <t>Hitech city</t>
   </si>
   <si>
@@ -118,9 +99,6 @@
     <t>Mpumalanga</t>
   </si>
   <si>
-    <t>salar@gmail.com</t>
-  </si>
-  <si>
     <t>Johannesburg</t>
   </si>
   <si>
@@ -1061,12 +1039,30 @@
       </rPr>
       <t>Nelspruit</t>
     </r>
+  </si>
+  <si>
+    <t>laddusi</t>
+  </si>
+  <si>
+    <t>garudasi</t>
+  </si>
+  <si>
+    <t>jv colony valli</t>
+  </si>
+  <si>
+    <t>siddque valli</t>
+  </si>
+  <si>
+    <t>goutiss11@gmail.com</t>
+  </si>
+  <si>
+    <t>salarjang11@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7">
     <font>
       <sz val="10"/>
@@ -1372,8 +1368,8 @@
   </sheetPr>
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
@@ -1383,7 +1379,7 @@
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="12" max="12" width="15.54296875" customWidth="1"/>
     <col min="13" max="13" width="14.54296875" customWidth="1"/>
-    <col min="15" max="15" width="18" customWidth="1"/>
+    <col min="15" max="15" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" customHeight="1">
@@ -1444,45 +1440,45 @@
         <v>4567788990</v>
       </c>
       <c r="D2" s="4">
-        <v>6567766554</v>
+        <v>6567700114</v>
       </c>
       <c r="E2" s="4">
-        <v>6787788990</v>
-      </c>
-      <c r="F2" s="4" t="s">
+        <v>6781100990</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="K2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="M2" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="N2">
         <v>5000</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>24</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>6789955445</v>
@@ -1491,40 +1487,40 @@
         <v>8762244556</v>
       </c>
       <c r="D3">
-        <v>6754455667</v>
+        <v>6754115007</v>
       </c>
       <c r="E3">
-        <v>5678844556</v>
-      </c>
-      <c r="F3" s="5" t="s">
+        <v>5678114006</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="N3">
         <v>5004</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1584,493 +1580,493 @@
   <sheetData>
     <row r="1" spans="1:1" ht="13.5">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="13.5">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.5">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="13.5">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="13.5">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="13.5">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="13.5">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="13.5">
       <c r="A8" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="13.5">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="13.5">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="13.5">
       <c r="A11" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="13.5">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="13.5">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="13.5">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="13.5">
       <c r="A15" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="13.5">
       <c r="A16" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="13.5">
       <c r="A17" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="13.5">
       <c r="A18" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="13.5">
       <c r="A20" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="13.5">
       <c r="A21" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="13.5">
       <c r="A22" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="13.5">
       <c r="A23" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="13.5">
       <c r="A24" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="13.5">
       <c r="A25" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="13.5">
       <c r="A26" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="13.5">
       <c r="A27" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="13.5">
       <c r="A28" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="13.5">
       <c r="A29" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="13.5">
       <c r="A30" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="13.5">
       <c r="A31" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="13.5">
       <c r="A32" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="13.5">
       <c r="A33" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="13.5">
       <c r="A34" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="13.5">
       <c r="A35" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="13.5">
       <c r="A36" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="13.5">
       <c r="A37" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="13.5">
       <c r="A38" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="13.5">
       <c r="A39" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="13.5">
       <c r="A40" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="13.5">
       <c r="A41" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="13.5">
       <c r="A42" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="13.5">
       <c r="A43" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="13.5">
       <c r="A44" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="13.5">
       <c r="A45" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="13.5">
       <c r="A46" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="13.5">
       <c r="A47" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="13.5">
       <c r="A48" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="13.5">
       <c r="A49" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="13.5">
       <c r="A50" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="13.5">
       <c r="A51" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="13.5">
       <c r="A52" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="13.5">
       <c r="A53" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="13.5">
       <c r="A54" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="13.5">
       <c r="A55" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="13.5">
       <c r="A56" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="13.5">
       <c r="A57" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="13.5">
       <c r="A58" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="13.5">
       <c r="A59" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="13.5">
       <c r="A60" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="13.5">
       <c r="A61" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="13.5">
       <c r="A62" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="13.5">
       <c r="A63" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="13.5">
       <c r="A64" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="13.5">
       <c r="A65" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="13.5">
       <c r="A66" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="13.5">
       <c r="A67" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="13.5">
       <c r="A68" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="13.5">
       <c r="A69" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="13.5">
       <c r="A70" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="13.5">
       <c r="A71" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="13.5">
       <c r="A72" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="13.5">
       <c r="A73" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F73" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="13.5">
       <c r="A74" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F74" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I74" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="13.5">
       <c r="A75" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="13.5">
       <c r="A76" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="13.5">
       <c r="A77" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="13.5">
       <c r="A78" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="13.5">
       <c r="A79" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="13.5">
       <c r="A80" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="13.5">
       <c r="A81" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="82" spans="1:1" ht="13.5">
       <c r="A82" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="13.5">
       <c r="A83" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="84" spans="1:1" ht="13.5">
       <c r="A84" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="13.5">
       <c r="A85" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="13.5">
       <c r="A86" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="13.5">
       <c r="A87" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="13.5">
       <c r="A88" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="13.5">
       <c r="A89" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="13.5">
       <c r="A90" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="91" spans="1:1" ht="13.5">
       <c r="A91" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit updated code on 05 June 2024
</commit_message>
<xml_diff>
--- a/Auto-IT/bulk_clients.xlsx
+++ b/Auto-IT/bulk_clients.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15530" windowHeight="6730"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14760" windowHeight="5860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="D1:L17"/>
 </workbook>
 </file>
 
@@ -67,18 +63,9 @@
     <t>email</t>
   </si>
   <si>
-    <t>seed.co</t>
-  </si>
-  <si>
-    <t>laddu</t>
-  </si>
-  <si>
     <t>Inactive</t>
   </si>
   <si>
-    <t>jv colony</t>
-  </si>
-  <si>
     <t>Gachibowli</t>
   </si>
   <si>
@@ -94,21 +81,9 @@
     <t>Eastern Cape</t>
   </si>
   <si>
-    <t>gouti@gmail.com</t>
-  </si>
-  <si>
-    <t>earth.co</t>
-  </si>
-  <si>
-    <t>garuda</t>
-  </si>
-  <si>
     <t>active</t>
   </si>
   <si>
-    <t>siddque</t>
-  </si>
-  <si>
     <t>Hitech city</t>
   </si>
   <si>
@@ -118,9 +93,6 @@
     <t>Mpumalanga</t>
   </si>
   <si>
-    <t>salar@gmail.com</t>
-  </si>
-  <si>
     <t>Johannesburg</t>
   </si>
   <si>
@@ -1061,12 +1033,36 @@
       </rPr>
       <t>Nelspruit</t>
     </r>
+  </si>
+  <si>
+    <t>laddusi</t>
+  </si>
+  <si>
+    <t>garudasi</t>
+  </si>
+  <si>
+    <t>jv colony valli</t>
+  </si>
+  <si>
+    <t>siddque valli</t>
+  </si>
+  <si>
+    <t>goutiss1234@gmail.com</t>
+  </si>
+  <si>
+    <t>salarjang1339@gmail.com</t>
+  </si>
+  <si>
+    <t>Ty.co</t>
+  </si>
+  <si>
+    <t>TYS.co</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7">
     <font>
       <sz val="10"/>
@@ -1372,8 +1368,8 @@
   </sheetPr>
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
@@ -1383,7 +1379,7 @@
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="12" max="12" width="15.54296875" customWidth="1"/>
     <col min="13" max="13" width="14.54296875" customWidth="1"/>
-    <col min="15" max="15" width="18" customWidth="1"/>
+    <col min="15" max="15" width="22.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" customHeight="1">
@@ -1434,8 +1430,8 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A2" s="4" t="s">
-        <v>15</v>
+      <c r="A2" s="3" t="s">
+        <v>129</v>
       </c>
       <c r="B2" s="4">
         <v>9098877665</v>
@@ -1444,45 +1440,45 @@
         <v>4567788990</v>
       </c>
       <c r="D2" s="4">
-        <v>6567766554</v>
+        <v>6567700114</v>
       </c>
       <c r="E2" s="4">
-        <v>6787788990</v>
-      </c>
-      <c r="F2" s="4" t="s">
+        <v>6781100990</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="K2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="M2" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="N2">
         <v>5000</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>24</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>25</v>
+      <c r="A3" s="7" t="s">
+        <v>130</v>
       </c>
       <c r="B3">
         <v>6789955445</v>
@@ -1491,40 +1487,40 @@
         <v>8762244556</v>
       </c>
       <c r="D3">
-        <v>6754455667</v>
+        <v>6754115007</v>
       </c>
       <c r="E3">
-        <v>5678844556</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>26</v>
+        <v>5678114006</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>124</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="K3" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="N3">
         <v>5004</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>32</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1584,493 +1580,493 @@
   <sheetData>
     <row r="1" spans="1:1" ht="13.5">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="13.5">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.5">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="13.5">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="13.5">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="13.5">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="13.5">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="13.5">
       <c r="A8" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="13.5">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="13.5">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="13.5">
       <c r="A11" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="13.5">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="13.5">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="13.5">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="13.5">
       <c r="A15" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="13.5">
       <c r="A16" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="13.5">
       <c r="A17" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="13.5">
       <c r="A18" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="13.5">
       <c r="A20" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="13.5">
       <c r="A21" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="13.5">
       <c r="A22" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="13.5">
       <c r="A23" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="13.5">
       <c r="A24" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="13.5">
       <c r="A25" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="13.5">
       <c r="A26" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="13.5">
       <c r="A27" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="13.5">
       <c r="A28" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="13.5">
       <c r="A29" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="13.5">
       <c r="A30" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="13.5">
       <c r="A31" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="13.5">
       <c r="A32" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="13.5">
       <c r="A33" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="13.5">
       <c r="A34" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="13.5">
       <c r="A35" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="13.5">
       <c r="A36" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="13.5">
       <c r="A37" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="13.5">
       <c r="A38" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="13.5">
       <c r="A39" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="13.5">
       <c r="A40" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="13.5">
       <c r="A41" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="13.5">
       <c r="A42" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="13.5">
       <c r="A43" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="13.5">
       <c r="A44" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="13.5">
       <c r="A45" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="13.5">
       <c r="A46" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="13.5">
       <c r="A47" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="13.5">
       <c r="A48" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="13.5">
       <c r="A49" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="13.5">
       <c r="A50" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="13.5">
       <c r="A51" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="13.5">
       <c r="A52" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="13.5">
       <c r="A53" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="13.5">
       <c r="A54" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="13.5">
       <c r="A55" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="13.5">
       <c r="A56" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="13.5">
       <c r="A57" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="13.5">
       <c r="A58" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="13.5">
       <c r="A59" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="13.5">
       <c r="A60" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="13.5">
       <c r="A61" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="13.5">
       <c r="A62" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="13.5">
       <c r="A63" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="13.5">
       <c r="A64" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="13.5">
       <c r="A65" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="13.5">
       <c r="A66" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="13.5">
       <c r="A67" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="13.5">
       <c r="A68" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="13.5">
       <c r="A69" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="13.5">
       <c r="A70" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="13.5">
       <c r="A71" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="13.5">
       <c r="A72" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="13.5">
       <c r="A73" s="1" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="F73" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="13.5">
       <c r="A74" s="1" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F74" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I74" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="13.5">
       <c r="A75" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="13.5">
       <c r="A76" s="1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="13.5">
       <c r="A77" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="13.5">
       <c r="A78" s="1" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="13.5">
       <c r="A79" s="1" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="13.5">
       <c r="A80" s="1" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="13.5">
       <c r="A81" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="82" spans="1:1" ht="13.5">
       <c r="A82" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="13.5">
       <c r="A83" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="84" spans="1:1" ht="13.5">
       <c r="A84" s="1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="13.5">
       <c r="A85" s="1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="13.5">
       <c r="A86" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="13.5">
       <c r="A87" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="13.5">
       <c r="A88" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="13.5">
       <c r="A89" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="13.5">
       <c r="A90" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="91" spans="1:1" ht="13.5">
       <c r="A91" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated scripts for resolving conflicts
</commit_message>
<xml_diff>
--- a/Auto-IT/bulk_clients.xlsx
+++ b/Auto-IT/bulk_clients.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14760" windowHeight="5860"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13630" windowHeight="5860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1047,16 +1047,16 @@
     <t>siddque valli</t>
   </si>
   <si>
-    <t>goutiss1234@gmail.com</t>
-  </si>
-  <si>
-    <t>salarjang1339@gmail.com</t>
-  </si>
-  <si>
-    <t>Ty.co</t>
-  </si>
-  <si>
-    <t>TYS.co</t>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>ABCS</t>
+  </si>
+  <si>
+    <t>ABC@gmail.com</t>
+  </si>
+  <si>
+    <t>ABCS@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1368,8 +1368,8 @@
   </sheetPr>
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
@@ -1379,7 +1379,7 @@
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="12" max="12" width="15.54296875" customWidth="1"/>
     <col min="13" max="13" width="14.54296875" customWidth="1"/>
-    <col min="15" max="15" width="22.08984375" customWidth="1"/>
+    <col min="15" max="15" width="24.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" customHeight="1">
@@ -1431,16 +1431,16 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B2" s="4">
-        <v>9098877665</v>
+        <v>9098833665</v>
       </c>
       <c r="C2" s="4">
-        <v>4567788990</v>
+        <v>4560783390</v>
       </c>
       <c r="D2" s="4">
-        <v>6567700114</v>
+        <v>6567701114</v>
       </c>
       <c r="E2" s="4">
         <v>6781100990</v>
@@ -1473,18 +1473,18 @@
         <v>5000</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B3">
-        <v>6789955445</v>
+        <v>6789933115</v>
       </c>
       <c r="C3">
-        <v>8762244556</v>
+        <v>8760243356</v>
       </c>
       <c r="D3">
         <v>6754115007</v>
@@ -1520,7 +1520,7 @@
         <v>5004</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated code on 14th June
</commit_message>
<xml_diff>
--- a/Auto-IT/bulk_clients.xlsx
+++ b/Auto-IT/bulk_clients.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14760" windowHeight="5860"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14330" windowHeight="5860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1047,16 +1047,16 @@
     <t>siddque valli</t>
   </si>
   <si>
-    <t>goutiss1234@gmail.com</t>
-  </si>
-  <si>
-    <t>salarjang1339@gmail.com</t>
-  </si>
-  <si>
-    <t>Ty.co</t>
-  </si>
-  <si>
-    <t>TYS.co</t>
+    <t>ABCD</t>
+  </si>
+  <si>
+    <t>ABCDS</t>
+  </si>
+  <si>
+    <t>ABCD@gmail.com</t>
+  </si>
+  <si>
+    <t>ABCDS@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1368,8 +1368,8 @@
   </sheetPr>
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
@@ -1379,7 +1379,7 @@
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="12" max="12" width="15.54296875" customWidth="1"/>
     <col min="13" max="13" width="14.54296875" customWidth="1"/>
-    <col min="15" max="15" width="22.08984375" customWidth="1"/>
+    <col min="15" max="15" width="24.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" customHeight="1">
@@ -1431,19 +1431,19 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B2" s="4">
-        <v>9098877665</v>
+        <v>9098833605</v>
       </c>
       <c r="C2" s="4">
-        <v>4567788990</v>
+        <v>4560783190</v>
       </c>
       <c r="D2" s="4">
         <v>6567700114</v>
       </c>
       <c r="E2" s="4">
-        <v>6781100990</v>
+        <v>6781000990</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>123</v>
@@ -1473,24 +1473,24 @@
         <v>5000</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B3">
-        <v>6789955445</v>
+        <v>6789933105</v>
       </c>
       <c r="C3">
-        <v>8762244556</v>
+        <v>8760243156</v>
       </c>
       <c r="D3">
-        <v>6754115007</v>
+        <v>6754110007</v>
       </c>
       <c r="E3">
-        <v>5678114006</v>
+        <v>5670114006</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>124</v>
@@ -1520,7 +1520,7 @@
         <v>5004</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
up to date code ready to push
</commit_message>
<xml_diff>
--- a/Auto-IT/bulk_clients.xlsx
+++ b/Auto-IT/bulk_clients.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13030" windowHeight="5860"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14220" windowHeight="6080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1053,16 +1053,16 @@
     <t>ABCDS</t>
   </si>
   <si>
-    <t>ABCD06@gmail.com</t>
-  </si>
-  <si>
-    <t>ABCDS07@gmail.com</t>
+    <t>Acc@gmail.com</t>
+  </si>
+  <si>
+    <t>ABcs1@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7">
     <font>
       <sz val="10"/>
@@ -1368,8 +1368,8 @@
   </sheetPr>
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
@@ -1473,7 +1473,7 @@
         <v>5000</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1">
@@ -1520,7 +1520,7 @@
         <v>5004</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>